<commit_message>
checks on data and code
</commit_message>
<xml_diff>
--- a/aek_checks/our_own_files/repo_files.xlsx
+++ b/aek_checks/our_own_files/repo_files.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\Research\Current_projects\with_Erin_Katja\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\orig_forecasting\repro-Forecasting_Tournament\aek_checks\our_own_files\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B6F3C5B-0166-4C51-94A0-8A636523404D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17AEC527-35B3-4E4A-A3B6-157FA6FA6B2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{612497B5-7F0E-459A-88BF-55DA318010A4}"/>
+    <workbookView xWindow="5220" yWindow="30" windowWidth="21600" windowHeight="17085" xr2:uid="{612497B5-7F0E-459A-88BF-55DA318010A4}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="445" uniqueCount="246">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="455" uniqueCount="247">
   <si>
     <t>DTW</t>
   </si>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>unclear what this file does and if it is needed. Not used by any of the other files in the repo</t>
+  </si>
+  <si>
+    <t>same name as a file in the root dir</t>
   </si>
 </sst>
 </file>
@@ -1160,10 +1163,10 @@
   <dimension ref="A1:K125"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="G2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="I15" sqref="I15"/>
+      <selection pane="bottomRight" activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" outlineLevelCol="1" x14ac:dyDescent="0.25"/>
@@ -1325,7 +1328,7 @@
         <v>230</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>9</v>
       </c>
@@ -1341,8 +1344,11 @@
       <c r="H10" s="1" t="s">
         <v>232</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" ht="45" x14ac:dyDescent="0.25">
+      <c r="I10" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="90" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>10</v>
       </c>
@@ -1357,6 +1363,9 @@
       </c>
       <c r="H11" s="1" t="s">
         <v>232</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="12" spans="1:11" x14ac:dyDescent="0.25">
@@ -1501,7 +1510,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="20" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>19</v>
       </c>
@@ -1513,6 +1522,9 @@
       </c>
       <c r="G20" s="1" t="s">
         <v>138</v>
+      </c>
+      <c r="I20" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="90" x14ac:dyDescent="0.25">
@@ -1569,7 +1581,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="24" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>23</v>
       </c>
@@ -1582,8 +1594,11 @@
       <c r="G24" s="1" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="25" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+      <c r="I24" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>24</v>
       </c>
@@ -1595,6 +1610,9 @@
       </c>
       <c r="G25" s="1" t="s">
         <v>138</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>238</v>
       </c>
     </row>
     <row r="26" spans="1:9" ht="30" x14ac:dyDescent="0.25">
@@ -1716,7 +1734,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="33" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="2">
         <v>32</v>
       </c>
@@ -1730,7 +1748,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="34" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A34" s="2">
         <v>33</v>
       </c>
@@ -1743,8 +1761,11 @@
       <c r="F34" s="1" t="s">
         <v>133</v>
       </c>
-    </row>
-    <row r="35" spans="1:7" ht="105" x14ac:dyDescent="0.25">
+      <c r="I34" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A35" s="2">
         <v>34</v>
       </c>
@@ -1757,8 +1778,11 @@
       <c r="F35" s="1" t="s">
         <v>134</v>
       </c>
-    </row>
-    <row r="36" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="I35" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="2">
         <v>35</v>
       </c>
@@ -1772,7 +1796,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="37" spans="1:7" ht="135" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" ht="135" x14ac:dyDescent="0.25">
       <c r="A37" s="2">
         <v>36</v>
       </c>
@@ -1786,7 +1810,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="2">
         <v>37</v>
       </c>
@@ -1800,7 +1824,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="2">
         <v>38</v>
       </c>
@@ -1814,7 +1838,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="40" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2">
         <v>39</v>
       </c>
@@ -1828,7 +1852,7 @@
         <v>144</v>
       </c>
     </row>
-    <row r="41" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="2">
         <v>40</v>
       </c>
@@ -1842,7 +1866,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="42" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A42" s="2">
         <v>41</v>
       </c>
@@ -1855,8 +1879,11 @@
       <c r="F42" s="1" t="s">
         <v>131</v>
       </c>
-    </row>
-    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I42" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="2">
         <v>42</v>
       </c>
@@ -1870,7 +1897,7 @@
         <v>139</v>
       </c>
     </row>
-    <row r="44" spans="1:7" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" ht="90" x14ac:dyDescent="0.25">
       <c r="A44" s="2">
         <v>43</v>
       </c>
@@ -1883,8 +1910,11 @@
       <c r="F44" s="1" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="45" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I44" s="1" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="2">
         <v>44</v>
       </c>
@@ -1895,7 +1925,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="2">
         <v>45</v>
       </c>
@@ -1909,7 +1939,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="2">
         <v>46</v>
       </c>
@@ -1923,7 +1953,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="2">
         <v>47</v>
       </c>
@@ -1937,7 +1967,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="2">
         <v>48</v>
       </c>
@@ -1950,8 +1980,11 @@
       <c r="D49" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="G49" s="1" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="2">
         <v>49</v>
       </c>
@@ -1965,7 +1998,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="2">
         <v>50</v>
       </c>
@@ -1979,7 +2012,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="2">
         <v>51</v>
       </c>
@@ -1993,7 +2026,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="2">
         <v>52</v>
       </c>
@@ -2007,7 +2040,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="2">
         <v>53</v>
       </c>
@@ -2021,7 +2054,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="2">
         <v>54</v>
       </c>
@@ -2035,7 +2068,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="2">
         <v>55</v>
       </c>
@@ -2049,7 +2082,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="2">
         <v>56</v>
       </c>
@@ -2063,7 +2096,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="2">
         <v>57</v>
       </c>
@@ -2077,7 +2110,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="2">
         <v>58</v>
       </c>
@@ -2091,7 +2124,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="60" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A60" s="2">
         <v>59</v>
       </c>
@@ -2105,7 +2138,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="2">
         <v>60</v>
       </c>
@@ -2119,7 +2152,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="2">
         <v>61</v>
       </c>
@@ -2133,7 +2166,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A63" s="2">
         <v>62</v>
       </c>
@@ -2147,7 +2180,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="2">
         <v>63</v>
       </c>

</xml_diff>